<commit_message>
Taxonomies and Kirsten analysis updates
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/EMDAT_HIP.xlsx
+++ b/Taxonomies/MostlyImpactData/EMDAT_HIP.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Disaster.Subsubtype</t>
   </si>
   <si>
-    <t xml:space="preserve">hazEM</t>
+    <t xml:space="preserve">hazAb</t>
   </si>
   <si>
     <t xml:space="preserve">haztype</t>
@@ -247,25 +247,7 @@
     <t xml:space="preserve">GH0013</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">GH0012,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">GH0013,GH0009,GH0010</t>
-    </r>
+    <t xml:space="preserve">GH0012,GH0013,GH0009,GH0010</t>
   </si>
   <si>
     <t xml:space="preserve">Hydrological</t>
@@ -301,25 +283,7 @@
     <t xml:space="preserve">MH0009</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MH0004,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MH0005,MH0006,MH0007,MH0008,MH0012</t>
-    </r>
+    <t xml:space="preserve">MH0004,MH0005,MH0006,MH0007,MH0008,MH0012</t>
   </si>
   <si>
     <t xml:space="preserve">hazhmterr</t>
@@ -331,25 +295,7 @@
     <t xml:space="preserve">Winter storm/Blizzard</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MH0051,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MH0052</t>
-    </r>
+    <t xml:space="preserve">MH0051,MH0052</t>
   </si>
   <si>
     <t xml:space="preserve">Mudslide</t>
@@ -397,49 +343,13 @@
     <t xml:space="preserve">ET</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MH0042,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MH0043</t>
-    </r>
+    <t xml:space="preserve">MH0042,MH0043</t>
   </si>
   <si>
     <t xml:space="preserve">Snow/Ice</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MH0037,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MH0038,MH0039</t>
-    </r>
+    <t xml:space="preserve">MH0037,MH0038,MH0039</t>
   </si>
   <si>
     <t xml:space="preserve">Storm</t>
@@ -481,25 +391,7 @@
     <t xml:space="preserve">Severe storm</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MH0001,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MH0002,MH0003,</t>
-    </r>
+    <t xml:space="preserve">MH0001,MH0002,MH0003,</t>
   </si>
   <si>
     <t xml:space="preserve">Hail</t>
@@ -535,25 +427,7 @@
     <t xml:space="preserve">Wind</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MH0054,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MH0060</t>
-    </r>
+    <t xml:space="preserve">MH0054,MH0060</t>
   </si>
   <si>
     <t xml:space="preserve">Extra-tropical storm</t>
@@ -568,46 +442,10 @@
     <t xml:space="preserve">MH0057</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">hazhmwind,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">hazhmprecip,hazhmconv,hazhmmarine</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MH0059,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MH0001,MH0002,MH0003,MH0027,MH0054,MH0060</t>
-    </r>
+    <t xml:space="preserve">hazhmwind,hazhmprecip,hazhmconv,hazhmmarine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MH0059,MH0001,MH0002,MH0003,MH0027,MH0054,MH0060</t>
   </si>
   <si>
     <t xml:space="preserve">Fog</t>
@@ -623,7 +461,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -660,12 +498,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -710,12 +542,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -731,12 +563,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -759,28 +587,28 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -803,10 +631,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -814,13 +642,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -828,13 +656,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -842,10 +670,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -853,13 +681,13 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -867,13 +695,13 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -881,16 +709,16 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -904,13 +732,13 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -924,13 +752,13 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -944,16 +772,16 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -967,16 +795,16 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -990,13 +818,13 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -1010,10 +838,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -1027,42 +855,42 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -1076,16 +904,16 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -1099,16 +927,16 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -1122,16 +950,16 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -1145,16 +973,16 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -1168,16 +996,16 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -1191,16 +1019,16 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -1214,16 +1042,16 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -1237,14 +1065,14 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -1258,16 +1086,16 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F25" s="3" t="s">
@@ -1281,16 +1109,16 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F26" s="3" t="s">
@@ -1304,16 +1132,16 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F27" s="3" t="s">
@@ -1327,16 +1155,16 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -1350,14 +1178,14 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F29" s="3" t="s">
@@ -1371,16 +1199,16 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F30" s="3" t="s">
@@ -1394,19 +1222,19 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F31" s="3" t="s">
@@ -1420,16 +1248,16 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F32" s="3" t="s">
@@ -1443,16 +1271,16 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F33" s="3" t="s">
@@ -1466,16 +1294,16 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F34" s="3" t="s">
@@ -1489,13 +1317,13 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F35" s="3" t="s">
@@ -1509,16 +1337,16 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="1" t="s">
         <v>98</v>
       </c>
       <c r="F36" s="3" t="s">
@@ -1532,16 +1360,16 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" s="1" t="s">
         <v>102</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -1555,19 +1383,19 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -1581,19 +1409,19 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F39" s="3" t="s">
@@ -1607,19 +1435,19 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="1" t="s">
         <v>113</v>
       </c>
       <c r="F40" s="3" t="s">
@@ -1633,19 +1461,19 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F41" s="3" t="s">
@@ -1659,19 +1487,19 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F42" s="3" t="s">
@@ -1685,19 +1513,19 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F43" s="3" t="s">
@@ -1706,24 +1534,24 @@
       <c r="G43" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="H43" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -1737,19 +1565,19 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F45" s="3" t="s">
@@ -1763,19 +1591,19 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F46" s="3" t="s">
@@ -1789,19 +1617,19 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F47" s="3" t="s">
@@ -1815,19 +1643,19 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="E48" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -1841,19 +1669,19 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="E49" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F49" s="3" t="s">
@@ -1867,16 +1695,16 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="E50" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F50" s="3" t="s">
@@ -1890,16 +1718,16 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E51" s="1" t="s">
         <v>113</v>
       </c>
       <c r="F51" s="3" t="s">
@@ -1913,13 +1741,13 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="0" t="s">
+      <c r="E52" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F52" s="3" t="s">
@@ -1933,10 +1761,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>142</v>
       </c>
       <c r="F53" s="3" t="s">

</xml_diff>

<commit_message>
ATTENTION REFACTORISATION: Overhaul of data dictionary, resulting in the renaming of tens of variables throughout the entire project... pray for the best!
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/EMDAT_HIP.xlsx
+++ b/Taxonomies/MostlyImpactData/EMDAT_HIP.xlsx
@@ -34,19 +34,143 @@
     <t xml:space="preserve">Disaster.Subsubtype</t>
   </si>
   <si>
-    <t xml:space="preserve">hazAb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">haztype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hazcluster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hazspec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hazpotlink</t>
+    <t xml:space="preserve">haz_Ab</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">haz</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">haz</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">cluster</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">haz</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">haz</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">potlink</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">hazlink</t>
@@ -461,7 +585,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -491,6 +615,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -555,7 +686,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -587,7 +718,7 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -598,7 +729,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Adding taxonomies for GLIDE & GDACS
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/EMDAT_HIP.xlsx
+++ b/Taxonomies/MostlyImpactData/EMDAT_HIP.xlsx
@@ -572,33 +572,34 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E50" activeCellId="0" sqref="E50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,8 +1783,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>